<commit_message>
Ajout données aléatoires dans template de test
</commit_message>
<xml_diff>
--- a/template_greve_test_50.xlsx
+++ b/template_greve_test_50.xlsx
@@ -565,58 +565,58 @@
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
         <is>
-          <t>Prénom1</t>
+          <t>Marie</t>
         </is>
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>Nom1</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="C4" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L4" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>Prénom2</t>
+          <t>Jean</t>
         </is>
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>Nom2</t>
+          <t>Bernard</t>
         </is>
       </c>
       <c r="C5" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>0</v>
@@ -625,10 +625,10 @@
         <v>0</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="5" t="n">
         <v>0</v>
@@ -640,49 +640,49 @@
         <v>0</v>
       </c>
       <c r="K5" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
         <is>
-          <t>Prénom3</t>
+          <t>Sophie</t>
         </is>
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>Nom3</t>
+          <t>Dubois</t>
         </is>
       </c>
       <c r="C6" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K6" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="5" t="n">
         <v>0</v>
@@ -691,124 +691,124 @@
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>Prénom4</t>
+          <t>Pierre</t>
         </is>
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t>Nom4</t>
+          <t>Thomas</t>
         </is>
       </c>
       <c r="C7" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
-          <t>Prénom5</t>
+          <t>Julie</t>
         </is>
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t>Nom5</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C8" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
         <is>
-          <t>Prénom6</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t>Nom6</t>
+          <t>Richard</t>
         </is>
       </c>
       <c r="C9" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J9" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="5" t="n">
         <v>0</v>
@@ -817,145 +817,145 @@
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
         <is>
-          <t>Prénom7</t>
+          <t>Laura</t>
         </is>
       </c>
       <c r="B10" s="4" t="inlineStr">
         <is>
-          <t>Nom7</t>
+          <t>Petit</t>
         </is>
       </c>
       <c r="C10" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L10" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>Prénom8</t>
+          <t>Thomas</t>
         </is>
       </c>
       <c r="B11" s="4" t="inlineStr">
         <is>
-          <t>Nom8</t>
+          <t>Durand</t>
         </is>
       </c>
       <c r="C11" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J11" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
         <is>
-          <t>Prénom9</t>
+          <t>Céline</t>
         </is>
       </c>
       <c r="B12" s="4" t="inlineStr">
         <is>
-          <t>Nom9</t>
+          <t>Leroy</t>
         </is>
       </c>
       <c r="C12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>Prénom10</t>
+          <t>Nicolas</t>
         </is>
       </c>
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t>Nom10</t>
+          <t>Moreau</t>
         </is>
       </c>
       <c r="C13" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>0</v>
@@ -973,7 +973,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="5" t="n">
         <v>0</v>
@@ -985,82 +985,82 @@
     <row r="14">
       <c r="A14" s="4" t="inlineStr">
         <is>
-          <t>Prénom11</t>
+          <t>Emma</t>
         </is>
       </c>
       <c r="B14" s="4" t="inlineStr">
         <is>
-          <t>Nom11</t>
+          <t>Simon</t>
         </is>
       </c>
       <c r="C14" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I14" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L14" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>Prénom12</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="B15" s="4" t="inlineStr">
         <is>
-          <t>Nom12</t>
+          <t>Laurent</t>
         </is>
       </c>
       <c r="C15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K15" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="5" t="n">
         <v>0</v>
@@ -1069,199 +1069,199 @@
     <row r="16">
       <c r="A16" s="4" t="inlineStr">
         <is>
-          <t>Prénom13</t>
+          <t>Camille</t>
         </is>
       </c>
       <c r="B16" s="4" t="inlineStr">
         <is>
-          <t>Nom13</t>
+          <t>Lefebvre</t>
         </is>
       </c>
       <c r="C16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="5" t="n">
         <v>0</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>Prénom14</t>
+          <t>Alexandre</t>
         </is>
       </c>
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t>Nom14</t>
+          <t>Michel</t>
         </is>
       </c>
       <c r="C17" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
         <is>
-          <t>Prénom15</t>
+          <t>Léa</t>
         </is>
       </c>
       <c r="B18" s="4" t="inlineStr">
         <is>
-          <t>Nom15</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="C18" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J18" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
         <is>
-          <t>Prénom16</t>
+          <t>Julien</t>
         </is>
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>Nom16</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C19" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K19" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>Prénom17</t>
+          <t>Sarah</t>
         </is>
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>Nom17</t>
+          <t>Bertrand</t>
         </is>
       </c>
       <c r="C20" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="5" t="n">
         <v>0</v>
@@ -1270,193 +1270,193 @@
         <v>0</v>
       </c>
       <c r="K20" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>Prénom18</t>
+          <t>Mathieu</t>
         </is>
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>Nom18</t>
+          <t>Roux</t>
         </is>
       </c>
       <c r="C21" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="5" t="n">
         <v>0</v>
       </c>
       <c r="G21" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>Prénom19</t>
+          <t>Chloé</t>
         </is>
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>Nom19</t>
+          <t>Vincent</t>
         </is>
       </c>
       <c r="C22" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="5" t="n">
         <v>0</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>Prénom20</t>
+          <t>David</t>
         </is>
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>Nom20</t>
+          <t>Fournier</t>
         </is>
       </c>
       <c r="C23" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H23" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="inlineStr">
         <is>
-          <t>Prénom21</t>
+          <t>Manon</t>
         </is>
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
-          <t>Nom21</t>
+          <t>Morel</t>
         </is>
       </c>
       <c r="C24" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L24" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="inlineStr">
         <is>
-          <t>Prénom22</t>
+          <t>Antoine</t>
         </is>
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>Nom22</t>
+          <t>Girard</t>
         </is>
       </c>
       <c r="C25" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="5" t="n">
         <v>0</v>
@@ -1465,64 +1465,64 @@
         <v>0</v>
       </c>
       <c r="F25" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L25" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="inlineStr">
         <is>
-          <t>Prénom23</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="B26" s="4" t="inlineStr">
         <is>
-          <t>Nom23</t>
+          <t>André</t>
         </is>
       </c>
       <c r="C26" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D26" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F26" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26" s="5" t="n">
         <v>0</v>
@@ -1531,37 +1531,37 @@
     <row r="27">
       <c r="A27" s="4" t="inlineStr">
         <is>
-          <t>Prénom24</t>
+          <t>Vincent</t>
         </is>
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>Nom24</t>
+          <t>Lefevre</t>
         </is>
       </c>
       <c r="C27" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="5" t="n">
         <v>0</v>
       </c>
       <c r="G27" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="5" t="n">
         <v>0</v>
@@ -1573,12 +1573,12 @@
     <row r="28">
       <c r="A28" s="4" t="inlineStr">
         <is>
-          <t>Prénom25</t>
+          <t>Lisa</t>
         </is>
       </c>
       <c r="B28" s="4" t="inlineStr">
         <is>
-          <t>Nom25</t>
+          <t>Mercier</t>
         </is>
       </c>
       <c r="C28" s="5" t="n">
@@ -1591,19 +1591,19 @@
         <v>0</v>
       </c>
       <c r="F28" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" s="5" t="n">
         <v>0</v>
@@ -1615,103 +1615,103 @@
     <row r="29">
       <c r="A29" s="4" t="inlineStr">
         <is>
-          <t>Prénom26</t>
+          <t>Maxime</t>
         </is>
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>Nom26</t>
+          <t>Dupont</t>
         </is>
       </c>
       <c r="C29" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D29" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K29" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L29" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="inlineStr">
         <is>
-          <t>Prénom27</t>
+          <t>Océane</t>
         </is>
       </c>
       <c r="B30" s="4" t="inlineStr">
         <is>
-          <t>Nom27</t>
+          <t>Lambert</t>
         </is>
       </c>
       <c r="C30" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D30" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I30" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="inlineStr">
         <is>
-          <t>Prénom28</t>
+          <t>Romain</t>
         </is>
       </c>
       <c r="B31" s="4" t="inlineStr">
         <is>
-          <t>Nom28</t>
+          <t>Bonnet</t>
         </is>
       </c>
       <c r="C31" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>0</v>
@@ -1723,127 +1723,127 @@
         <v>0</v>
       </c>
       <c r="H31" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J31" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L31" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="inlineStr">
         <is>
-          <t>Prénom29</t>
+          <t>Eva</t>
         </is>
       </c>
       <c r="B32" s="4" t="inlineStr">
         <is>
-          <t>Nom29</t>
+          <t>François</t>
         </is>
       </c>
       <c r="C32" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D32" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="5" t="n">
         <v>0</v>
       </c>
       <c r="G32" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J32" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L32" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
         <is>
-          <t>Prénom30</t>
+          <t>Benjamin</t>
         </is>
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>Nom30</t>
+          <t>Martinez</t>
         </is>
       </c>
       <c r="C33" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="5" t="n">
         <v>0</v>
       </c>
       <c r="G33" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I33" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L33" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="4" t="inlineStr">
         <is>
-          <t>Prénom31</t>
+          <t>Alice</t>
         </is>
       </c>
       <c r="B34" s="4" t="inlineStr">
         <is>
-          <t>Nom31</t>
+          <t>Legrand</t>
         </is>
       </c>
       <c r="C34" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="5" t="n">
         <v>0</v>
@@ -1852,13 +1852,13 @@
         <v>0</v>
       </c>
       <c r="I34" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K34" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34" s="5" t="n">
         <v>0</v>
@@ -1867,40 +1867,40 @@
     <row r="35">
       <c r="A35" s="4" t="inlineStr">
         <is>
-          <t>Prénom32</t>
+          <t>François</t>
         </is>
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>Nom32</t>
+          <t>Garnier</t>
         </is>
       </c>
       <c r="C35" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D35" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L35" s="5" t="n">
         <v>0</v>
@@ -1909,118 +1909,118 @@
     <row r="36">
       <c r="A36" s="4" t="inlineStr">
         <is>
-          <t>Prénom33</t>
+          <t>Clara</t>
         </is>
       </c>
       <c r="B36" s="4" t="inlineStr">
         <is>
-          <t>Nom33</t>
+          <t>Faure</t>
         </is>
       </c>
       <c r="C36" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D36" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F36" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J36" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L36" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="4" t="inlineStr">
         <is>
-          <t>Prénom34</t>
+          <t>Hugo</t>
         </is>
       </c>
       <c r="B37" s="4" t="inlineStr">
         <is>
-          <t>Nom34</t>
+          <t>Rousseau</t>
         </is>
       </c>
       <c r="C37" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="5" t="n">
         <v>0</v>
       </c>
       <c r="G37" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L37" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="inlineStr">
         <is>
-          <t>Prénom35</t>
+          <t>Inès</t>
         </is>
       </c>
       <c r="B38" s="4" t="inlineStr">
         <is>
-          <t>Nom35</t>
+          <t>Blanc</t>
         </is>
       </c>
       <c r="C38" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" s="5" t="n">
         <v>0</v>
@@ -2029,22 +2029,22 @@
         <v>0</v>
       </c>
       <c r="L38" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
         <is>
-          <t>Prénom36</t>
+          <t>Arthur</t>
         </is>
       </c>
       <c r="B39" s="4" t="inlineStr">
         <is>
-          <t>Nom36</t>
+          <t>Guerin</t>
         </is>
       </c>
       <c r="C39" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" s="5" t="n">
         <v>0</v>
@@ -2056,19 +2056,19 @@
         <v>0</v>
       </c>
       <c r="G39" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K39" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L39" s="5" t="n">
         <v>0</v>
@@ -2077,37 +2077,37 @@
     <row r="40">
       <c r="A40" s="4" t="inlineStr">
         <is>
-          <t>Prénom37</t>
+          <t>Jade</t>
         </is>
       </c>
       <c r="B40" s="4" t="inlineStr">
         <is>
-          <t>Nom37</t>
+          <t>Muller</t>
         </is>
       </c>
       <c r="C40" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F40" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K40" s="5" t="n">
         <v>0</v>
@@ -2119,16 +2119,16 @@
     <row r="41">
       <c r="A41" s="4" t="inlineStr">
         <is>
-          <t>Prénom38</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="B41" s="4" t="inlineStr">
         <is>
-          <t>Nom38</t>
+          <t>Henry</t>
         </is>
       </c>
       <c r="C41" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" s="5" t="n">
         <v>0</v>
@@ -2140,97 +2140,97 @@
         <v>0</v>
       </c>
       <c r="G41" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K41" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="4" t="inlineStr">
         <is>
-          <t>Prénom39</t>
+          <t>Anaïs</t>
         </is>
       </c>
       <c r="B42" s="4" t="inlineStr">
         <is>
-          <t>Nom39</t>
+          <t>Roussel</t>
         </is>
       </c>
       <c r="C42" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I42" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L42" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="4" t="inlineStr">
         <is>
-          <t>Prénom40</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="B43" s="4" t="inlineStr">
         <is>
-          <t>Nom40</t>
+          <t>Nicolas</t>
         </is>
       </c>
       <c r="C43" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D43" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H43" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" s="5" t="n">
         <v>0</v>
@@ -2245,82 +2245,82 @@
     <row r="44">
       <c r="A44" s="4" t="inlineStr">
         <is>
-          <t>Prénom41</t>
+          <t>Lucie</t>
         </is>
       </c>
       <c r="B44" s="4" t="inlineStr">
         <is>
-          <t>Nom41</t>
+          <t>Perrin</t>
         </is>
       </c>
       <c r="C44" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D44" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44" s="5" t="n">
         <v>0</v>
       </c>
       <c r="I44" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L44" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="4" t="inlineStr">
         <is>
-          <t>Prénom42</t>
+          <t>Simon</t>
         </is>
       </c>
       <c r="B45" s="4" t="inlineStr">
         <is>
-          <t>Nom42</t>
+          <t>Morin</t>
         </is>
       </c>
       <c r="C45" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K45" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L45" s="5" t="n">
         <v>0</v>
@@ -2329,25 +2329,25 @@
     <row r="46">
       <c r="A46" s="4" t="inlineStr">
         <is>
-          <t>Prénom43</t>
+          <t>Margot</t>
         </is>
       </c>
       <c r="B46" s="4" t="inlineStr">
         <is>
-          <t>Nom43</t>
+          <t>Mathieu</t>
         </is>
       </c>
       <c r="C46" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="5" t="n">
         <v>0</v>
@@ -2356,37 +2356,37 @@
         <v>0</v>
       </c>
       <c r="I46" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K46" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L46" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="4" t="inlineStr">
         <is>
-          <t>Prénom44</t>
+          <t>Gabriel</t>
         </is>
       </c>
       <c r="B47" s="4" t="inlineStr">
         <is>
-          <t>Nom44</t>
+          <t>Clement</t>
         </is>
       </c>
       <c r="C47" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D47" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" s="5" t="n">
         <v>0</v>
@@ -2398,94 +2398,94 @@
         <v>0</v>
       </c>
       <c r="I47" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L47" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="4" t="inlineStr">
         <is>
-          <t>Prénom45</t>
+          <t>Zoé</t>
         </is>
       </c>
       <c r="B48" s="4" t="inlineStr">
         <is>
-          <t>Nom45</t>
+          <t>Gauthier</t>
         </is>
       </c>
       <c r="C48" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D48" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F48" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H48" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I48" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J48" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K48" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L48" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="4" t="inlineStr">
         <is>
-          <t>Prénom46</t>
+          <t>Raphaël</t>
         </is>
       </c>
       <c r="B49" s="4" t="inlineStr">
         <is>
-          <t>Nom46</t>
+          <t>Dumont</t>
         </is>
       </c>
       <c r="C49" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F49" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K49" s="5" t="n">
         <v>0</v>
@@ -2497,37 +2497,37 @@
     <row r="50">
       <c r="A50" s="4" t="inlineStr">
         <is>
-          <t>Prénom47</t>
+          <t>Louise</t>
         </is>
       </c>
       <c r="B50" s="4" t="inlineStr">
         <is>
-          <t>Nom47</t>
+          <t>Lopez</t>
         </is>
       </c>
       <c r="C50" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D50" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K50" s="5" t="n">
         <v>0</v>
@@ -2539,25 +2539,25 @@
     <row r="51">
       <c r="A51" s="4" t="inlineStr">
         <is>
-          <t>Prénom48</t>
+          <t>Tom</t>
         </is>
       </c>
       <c r="B51" s="4" t="inlineStr">
         <is>
-          <t>Nom48</t>
+          <t>Fontaine</t>
         </is>
       </c>
       <c r="C51" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E51" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G51" s="5" t="n">
         <v>0</v>
@@ -2566,27 +2566,27 @@
         <v>0</v>
       </c>
       <c r="I51" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" s="5" t="n">
         <v>0</v>
       </c>
       <c r="K51" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L51" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="4" t="inlineStr">
         <is>
-          <t>Prénom49</t>
+          <t>Lina</t>
         </is>
       </c>
       <c r="B52" s="4" t="inlineStr">
         <is>
-          <t>Nom49</t>
+          <t>Chevalier</t>
         </is>
       </c>
       <c r="C52" s="5" t="n">
@@ -2596,22 +2596,22 @@
         <v>0</v>
       </c>
       <c r="E52" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G52" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K52" s="5" t="n">
         <v>0</v>
@@ -2623,43 +2623,43 @@
     <row r="53">
       <c r="A53" s="4" t="inlineStr">
         <is>
-          <t>Prénom50</t>
+          <t>Nathan</t>
         </is>
       </c>
       <c r="B53" s="4" t="inlineStr">
         <is>
-          <t>Nom50</t>
+          <t>Robin</t>
         </is>
       </c>
       <c r="C53" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>0</v>
       </c>
       <c r="F53" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H53" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J53" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K53" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L53" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">

</xml_diff>